<commit_message>
Import data from excel file and apply data cleaning code
</commit_message>
<xml_diff>
--- a/test/test_data.xlsx
+++ b/test/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/dev/prive/tessa/alignement_cognats/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tessavermeir/dev/alignement_cognats/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708AB019-6D22-C845-8EAA-AC4D7B13A2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B7820B-93E7-8848-A9EF-21C30FB1FBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="880" windowWidth="24840" windowHeight="15500" xr2:uid="{1D769B08-90E3-1F4F-900C-4DDAF00F6F14}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="24840" windowHeight="15500" xr2:uid="{1D769B08-90E3-1F4F-900C-4DDAF00F6F14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -758,7 +758,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -775,7 +775,7 @@
     <col min="13" max="13" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="52" thickBot="1">
+    <row r="1" spans="1:19" ht="70" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -826,7 +826,7 @@
       </c>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:19" ht="41.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:19" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="35" thickBot="1">
+    <row r="3" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -922,7 +922,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="35" thickBot="1">
+    <row r="4" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -975,7 +975,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="35" thickBot="1">
+    <row r="5" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:19" ht="24" customHeight="1" thickBot="1">
+    <row r="6" spans="1:19" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" ht="35" thickBot="1">
+    <row r="7" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="R7" s="3"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:19" ht="35" thickBot="1">
+    <row r="8" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" ht="18" thickBot="1">
+    <row r="9" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1231,7 +1231,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:19" ht="18" thickBot="1">
+    <row r="10" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>58</v>
       </c>
@@ -1281,43 +1281,43 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" ht="22" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" ht="22" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" ht="22" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" ht="22" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" ht="22" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
     </row>
   </sheetData>

</xml_diff>